<commit_message>
Data cleanup, transformation script started
</commit_message>
<xml_diff>
--- a/financial-empowerment/Copy of SMN_Filter Template_All Organizations_To merge_KN.xlsx
+++ b/financial-empowerment/Copy of SMN_Filter Template_All Organizations_To merge_KN.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="30" windowWidth="28725" windowHeight="11295" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="services.csv" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="483">
   <si>
     <t>Name of Service or Product</t>
   </si>
@@ -1514,12 +1519,81 @@
     <t>1325-B Evans Avenue
 San Francisco, CA 94124</t>
   </si>
+  <si>
+    <t>595 Market Street, 16th Floor
+San Francisco, CA 94105</t>
+  </si>
+  <si>
+    <t>3269 Mission Street
+San Francisco, CA 94110</t>
+  </si>
+  <si>
+    <t>7677 Oakport St. Ste. 1130
+Oakland, CA 94621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3062 East 9th Street
+Oakland, California 94601 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1215 Prytania Street Suite 103
+New Orleans, Louisiana 70130 </t>
+  </si>
+  <si>
+    <t>275 5th Steet
+San Francisco, California, 94103</t>
+  </si>
+  <si>
+    <t>2121 N. California Blvd. Suite 395
+Walnut Creek, CA 94596</t>
+  </si>
+  <si>
+    <t>1800 Market Street
+San Francisco, CA 94102</t>
+  </si>
+  <si>
+    <t>1825 Park Avenue, Suite 503
+New York, NY 10035</t>
+  </si>
+  <si>
+    <t>3300 College Dr. 
+San Bruno, CA 94066</t>
+  </si>
+  <si>
+    <t>840 West Orange Ave.
+South San Francisco, California</t>
+  </si>
+  <si>
+    <t>595 Market Street, 15th Floor
+San Francisco CA 94105</t>
+  </si>
+  <si>
+    <t>Plaza Adelante
+2301 Mission St., Suite 301
+San Francisco, CA 94110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 South Van Ness, 5th Fl
+San Francisco, CA 94103 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 South Van Ness, 5th Fl.
+San Francisco, CA 94103 </t>
+  </si>
+  <si>
+    <t>5030 Business Center Drive, Suite 260
+Fairfield, CA 94534</t>
+  </si>
+  <si>
+    <t>1470 Valencia Street
+San Francisco, California, 94110</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1623,6 +1697,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1654,26 +1736,36 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1760,7 +1852,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="12">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2053,20 +2155,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.85546875" customWidth="1"/>
+    <col min="17" max="17" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1">
@@ -2209,47 +2311,52 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="S3" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="D3" sqref="A1:Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="37.5">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2329,7 +2436,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="112.5">
+    <row r="2" spans="1:26" ht="90">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -2401,7 +2508,7 @@
       </c>
       <c r="Z2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="37.5">
+    <row r="3" spans="1:26" ht="36">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
@@ -2475,7 +2582,7 @@
       <c r="Y3" s="4"/>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="18.75">
+    <row r="4" spans="1:26" ht="18">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -2505,7 +2612,7 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="18.75">
+    <row r="5" spans="1:26" ht="18">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -2535,7 +2642,7 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="7"/>
     </row>
-    <row r="6" spans="1:26" ht="18.75">
+    <row r="6" spans="1:26" ht="18">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -2565,7 +2672,7 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:26" ht="18.75">
+    <row r="7" spans="1:26" ht="18">
       <c r="A7" s="8" t="s">
         <v>45</v>
       </c>
@@ -2601,50 +2708,55 @@
     <hyperlink ref="K3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ20"/>
   <sheetViews>
-    <sheetView topLeftCell="Z11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection sqref="A1:BQ20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.28515625" customWidth="1"/>
-    <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.33203125" customWidth="1"/>
+    <col min="10" max="10" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="43" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="34" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="64.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="144.75">
+    <row r="1" spans="1:69" ht="126">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2853,7 +2965,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="2" spans="1:69" ht="409.5">
+    <row r="2" spans="1:69" ht="409">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3054,7 +3166,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="3" spans="1:69" ht="187.5">
+    <row r="3" spans="1:69" ht="162">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -3243,7 +3355,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:69" ht="225">
+    <row r="4" spans="1:69" ht="180">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -3430,7 +3542,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="5" spans="1:69" ht="187.5">
+    <row r="5" spans="1:69" ht="162">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -3537,7 +3649,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:69" ht="112.5">
+    <row r="6" spans="1:69" ht="108">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3734,7 +3846,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="7" spans="1:69" ht="409.5">
+    <row r="7" spans="1:69" ht="409">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -3927,7 +4039,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="8" spans="1:69" ht="409.5">
+    <row r="8" spans="1:69" ht="409">
       <c r="A8" s="2" t="s">
         <v>58</v>
       </c>
@@ -4090,7 +4202,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="9" spans="1:69" ht="281.25">
+    <row r="9" spans="1:69" ht="216">
       <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
@@ -4175,7 +4287,7 @@
       <c r="BP9" s="10"/>
       <c r="BQ9" s="10"/>
     </row>
-    <row r="10" spans="1:69" ht="409.5">
+    <row r="10" spans="1:69" ht="409">
       <c r="A10" s="2" t="s">
         <v>69</v>
       </c>
@@ -4360,7 +4472,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:69" ht="150">
+    <row r="11" spans="1:69" ht="126">
       <c r="A11" s="2" t="s">
         <v>70</v>
       </c>
@@ -4483,7 +4595,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="12" spans="1:69" ht="409.5">
+    <row r="12" spans="1:69" ht="396">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -4660,7 +4772,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:69" ht="18.75">
+    <row r="13" spans="1:69" ht="18">
       <c r="A13" s="2" t="s">
         <v>72</v>
       </c>
@@ -4861,7 +4973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:69" ht="37.5">
+    <row r="14" spans="1:69" ht="18">
       <c r="A14" s="2" t="s">
         <v>73</v>
       </c>
@@ -5062,7 +5174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:69" ht="18.75">
+    <row r="15" spans="1:69" ht="18">
       <c r="A15" s="2" t="s">
         <v>74</v>
       </c>
@@ -5263,7 +5375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:69" ht="37.5">
+    <row r="16" spans="1:69" ht="18">
       <c r="A16" s="2" t="s">
         <v>75</v>
       </c>
@@ -5464,7 +5576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:69" ht="37.5">
+    <row r="17" spans="1:69" ht="36">
       <c r="A17" s="2" t="s">
         <v>76</v>
       </c>
@@ -5665,7 +5777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:69" ht="37.5">
+    <row r="18" spans="1:69" ht="18">
       <c r="A18" s="2" t="s">
         <v>77</v>
       </c>
@@ -5866,7 +5978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:69" ht="300">
+    <row r="19" spans="1:69" ht="270">
       <c r="A19" s="3" t="s">
         <v>80</v>
       </c>
@@ -5957,7 +6069,7 @@
       </c>
       <c r="BQ19" s="17"/>
     </row>
-    <row r="20" spans="1:69" ht="18.75">
+    <row r="20" spans="1:69" ht="18">
       <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
@@ -5992,31 +6104,38 @@
     <hyperlink ref="BQ6" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" customWidth="1"/>
+    <col min="8" max="8" width="45.5" customWidth="1"/>
+    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="10" max="10" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="131.25">
+    <row r="1" spans="1:20" ht="126">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6078,7 +6197,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="409.5">
+    <row r="2" spans="1:20" ht="409">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -6140,7 +6259,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="409.5">
+    <row r="3" spans="1:20" ht="144">
       <c r="A3" s="10" t="s">
         <v>82</v>
       </c>
@@ -6151,7 +6270,7 @@
         <v>92</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>93</v>
+        <v>466</v>
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="29" t="s">
@@ -6191,7 +6310,7 @@
       </c>
       <c r="S3" s="35"/>
     </row>
-    <row r="4" spans="1:20" ht="409.5">
+    <row r="4" spans="1:20" ht="180">
       <c r="A4" s="10" t="s">
         <v>83</v>
       </c>
@@ -6202,7 +6321,7 @@
         <v>92</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>93</v>
+        <v>466</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="29" t="s">
@@ -6242,7 +6361,7 @@
       </c>
       <c r="S4" s="35"/>
     </row>
-    <row r="5" spans="1:20" ht="409.5">
+    <row r="5" spans="1:20" ht="144">
       <c r="A5" s="10" t="s">
         <v>84</v>
       </c>
@@ -6253,7 +6372,7 @@
         <v>92</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>93</v>
+        <v>466</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="29" t="s">
@@ -6293,7 +6412,7 @@
       </c>
       <c r="S5" s="35"/>
     </row>
-    <row r="6" spans="1:20" ht="409.5">
+    <row r="6" spans="1:20" ht="108">
       <c r="A6" s="10" t="s">
         <v>85</v>
       </c>
@@ -6304,7 +6423,7 @@
         <v>92</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>93</v>
+        <v>466</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="29" t="s">
@@ -6344,7 +6463,7 @@
       </c>
       <c r="S6" s="35"/>
     </row>
-    <row r="7" spans="1:20" ht="409.5">
+    <row r="7" spans="1:20" ht="108">
       <c r="A7" s="11" t="s">
         <v>86</v>
       </c>
@@ -6355,7 +6474,7 @@
         <v>92</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>93</v>
+        <v>466</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="29" t="s">
@@ -6395,7 +6514,7 @@
       </c>
       <c r="S7" s="35"/>
     </row>
-    <row r="8" spans="1:20" ht="409.5">
+    <row r="8" spans="1:20" ht="90">
       <c r="A8" s="12" t="s">
         <v>104</v>
       </c>
@@ -6446,7 +6565,7 @@
       </c>
       <c r="S8" s="36"/>
     </row>
-    <row r="9" spans="1:20" ht="243.75">
+    <row r="9" spans="1:20" ht="198">
       <c r="A9" s="13" t="s">
         <v>113</v>
       </c>
@@ -6459,9 +6578,7 @@
       <c r="D9" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>119</v>
-      </c>
+      <c r="E9" s="26"/>
       <c r="F9" s="13" t="s">
         <v>116</v>
       </c>
@@ -6499,7 +6616,7 @@
       </c>
       <c r="S9" s="36"/>
     </row>
-    <row r="10" spans="1:20" ht="243.75">
+    <row r="10" spans="1:20" ht="198">
       <c r="A10" s="12" t="s">
         <v>31</v>
       </c>
@@ -6552,7 +6669,7 @@
       </c>
       <c r="S10" s="36"/>
     </row>
-    <row r="11" spans="1:20" ht="300">
+    <row r="11" spans="1:20" ht="144">
       <c r="A11" s="12" t="s">
         <v>120</v>
       </c>
@@ -6565,9 +6682,7 @@
       <c r="D11" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>127</v>
-      </c>
+      <c r="E11" s="12"/>
       <c r="F11" s="30" t="s">
         <v>129</v>
       </c>
@@ -6607,7 +6722,7 @@
       </c>
       <c r="S11" s="36"/>
     </row>
-    <row r="12" spans="1:20" ht="187.5">
+    <row r="12" spans="1:20" ht="144">
       <c r="A12" s="12" t="s">
         <v>121</v>
       </c>
@@ -6618,11 +6733,9 @@
         <v>125</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>128</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="E12" s="12"/>
       <c r="F12" s="30" t="s">
         <v>129</v>
       </c>
@@ -6662,7 +6775,7 @@
       </c>
       <c r="S12" s="36"/>
     </row>
-    <row r="13" spans="1:20" ht="409.5">
+    <row r="13" spans="1:20" ht="72">
       <c r="A13" s="10" t="s">
         <v>137</v>
       </c>
@@ -6676,7 +6789,7 @@
         <v>140</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>141</v>
+        <v>481</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>142</v>
@@ -6715,7 +6828,7 @@
       </c>
       <c r="S13" s="36"/>
     </row>
-    <row r="14" spans="1:20" ht="409.5">
+    <row r="14" spans="1:20" ht="126">
       <c r="A14" s="12" t="s">
         <v>147</v>
       </c>
@@ -6766,7 +6879,7 @@
       </c>
       <c r="S14" s="36"/>
     </row>
-    <row r="15" spans="1:20" ht="409.5">
+    <row r="15" spans="1:20" ht="72">
       <c r="A15" s="10" t="s">
         <v>155</v>
       </c>
@@ -6815,7 +6928,7 @@
       </c>
       <c r="S15" s="36"/>
     </row>
-    <row r="16" spans="1:20" ht="409.5">
+    <row r="16" spans="1:20" ht="54">
       <c r="A16" s="12" t="s">
         <v>163</v>
       </c>
@@ -6826,9 +6939,7 @@
         <v>165</v>
       </c>
       <c r="D16" s="12"/>
-      <c r="E16" s="12" t="s">
-        <v>166</v>
-      </c>
+      <c r="E16" s="12"/>
       <c r="F16" s="30" t="s">
         <v>167</v>
       </c>
@@ -6862,7 +6973,7 @@
       </c>
       <c r="S16" s="36"/>
     </row>
-    <row r="17" spans="1:19" ht="409.5">
+    <row r="17" spans="1:19" ht="162">
       <c r="A17" s="10" t="s">
         <v>169</v>
       </c>
@@ -6873,7 +6984,7 @@
         <v>173</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>174</v>
+        <v>467</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="29" t="s">
@@ -6911,7 +7022,7 @@
       </c>
       <c r="S17" s="36"/>
     </row>
-    <row r="18" spans="1:19" ht="409.5">
+    <row r="18" spans="1:19" ht="90">
       <c r="A18" s="10" t="s">
         <v>170</v>
       </c>
@@ -6922,7 +7033,7 @@
         <v>173</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>174</v>
+        <v>467</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="29" t="s">
@@ -6960,7 +7071,7 @@
       </c>
       <c r="S18" s="36"/>
     </row>
-    <row r="19" spans="1:19" ht="409.5">
+    <row r="19" spans="1:19" ht="126">
       <c r="A19" s="12" t="s">
         <v>181</v>
       </c>
@@ -6971,11 +7082,9 @@
         <v>189</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>184</v>
-      </c>
+        <v>468</v>
+      </c>
+      <c r="E19" s="12"/>
       <c r="F19" s="24" t="s">
         <v>185</v>
       </c>
@@ -7013,7 +7122,7 @@
       </c>
       <c r="S19" s="36"/>
     </row>
-    <row r="20" spans="1:19" ht="409.5">
+    <row r="20" spans="1:19" ht="162">
       <c r="A20" s="10" t="s">
         <v>190</v>
       </c>
@@ -7024,7 +7133,7 @@
         <v>200</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>203</v>
+        <v>469</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="29" t="s">
@@ -7064,7 +7173,7 @@
       </c>
       <c r="S20" s="17"/>
     </row>
-    <row r="21" spans="1:19" ht="409.5">
+    <row r="21" spans="1:19" ht="144">
       <c r="A21" s="10" t="s">
         <v>191</v>
       </c>
@@ -7075,7 +7184,7 @@
         <v>200</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>203</v>
+        <v>469</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="29" t="s">
@@ -7115,7 +7224,7 @@
       </c>
       <c r="S21" s="17"/>
     </row>
-    <row r="22" spans="1:19" ht="409.5">
+    <row r="22" spans="1:19" ht="216">
       <c r="A22" s="10" t="s">
         <v>192</v>
       </c>
@@ -7123,10 +7232,10 @@
         <v>197</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>204</v>
+        <v>470</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="29" t="s">
@@ -7162,7 +7271,7 @@
       </c>
       <c r="S22" s="17"/>
     </row>
-    <row r="23" spans="1:19" ht="225">
+    <row r="23" spans="1:19" ht="162">
       <c r="A23" s="10" t="s">
         <v>193</v>
       </c>
@@ -7170,11 +7279,9 @@
         <v>198</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>205</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D23" s="10"/>
       <c r="E23" s="29"/>
       <c r="F23" s="29" t="s">
         <v>206</v>
@@ -7213,7 +7320,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="409.5">
+    <row r="24" spans="1:19" ht="198">
       <c r="A24" s="12" t="s">
         <v>223</v>
       </c>
@@ -7224,7 +7331,7 @@
         <v>238</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>239</v>
+        <v>471</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="30" t="s">
@@ -7266,7 +7373,7 @@
       </c>
       <c r="S24" s="36"/>
     </row>
-    <row r="25" spans="1:19" ht="409.5">
+    <row r="25" spans="1:19" ht="108">
       <c r="A25" s="12" t="s">
         <v>224</v>
       </c>
@@ -7277,7 +7384,7 @@
         <v>238</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>239</v>
+        <v>471</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="30" t="s">
@@ -7317,7 +7424,7 @@
       </c>
       <c r="S25" s="36"/>
     </row>
-    <row r="26" spans="1:19" ht="409.5">
+    <row r="26" spans="1:19" ht="108">
       <c r="A26" s="12" t="s">
         <v>225</v>
       </c>
@@ -7328,7 +7435,7 @@
         <v>238</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>239</v>
+        <v>471</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="30" t="s">
@@ -7368,7 +7475,7 @@
       </c>
       <c r="S26" s="36"/>
     </row>
-    <row r="27" spans="1:19" ht="409.5">
+    <row r="27" spans="1:19" ht="108">
       <c r="A27" s="12" t="s">
         <v>226</v>
       </c>
@@ -7379,7 +7486,7 @@
         <v>238</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>239</v>
+        <v>471</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="30" t="s">
@@ -7419,7 +7526,7 @@
       </c>
       <c r="S27" s="36"/>
     </row>
-    <row r="28" spans="1:19" ht="409.5">
+    <row r="28" spans="1:19" ht="144">
       <c r="A28" s="14" t="s">
         <v>227</v>
       </c>
@@ -7430,7 +7537,7 @@
         <v>238</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>239</v>
+        <v>471</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="30" t="s">
@@ -7468,7 +7575,7 @@
       </c>
       <c r="S28" s="36"/>
     </row>
-    <row r="29" spans="1:19" ht="409.5">
+    <row r="29" spans="1:19" ht="162">
       <c r="A29" s="12" t="s">
         <v>228</v>
       </c>
@@ -7479,7 +7586,7 @@
         <v>238</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>240</v>
+        <v>465</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="31" t="s">
@@ -7519,7 +7626,7 @@
       </c>
       <c r="S29" s="36"/>
     </row>
-    <row r="30" spans="1:19" ht="409.5">
+    <row r="30" spans="1:19" ht="126">
       <c r="A30" s="12" t="s">
         <v>229</v>
       </c>
@@ -7530,7 +7637,7 @@
         <v>238</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>240</v>
+        <v>465</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="30" t="s">
@@ -7564,7 +7671,7 @@
       </c>
       <c r="S30" s="36"/>
     </row>
-    <row r="31" spans="1:19" ht="168.75">
+    <row r="31" spans="1:19" ht="144">
       <c r="A31" s="12" t="s">
         <v>47</v>
       </c>
@@ -7617,7 +7724,7 @@
       </c>
       <c r="S31" s="36"/>
     </row>
-    <row r="32" spans="1:19" ht="409.5">
+    <row r="32" spans="1:19" ht="108">
       <c r="A32" s="10" t="s">
         <v>266</v>
       </c>
@@ -7628,11 +7735,9 @@
         <v>272</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>274</v>
-      </c>
+        <v>472</v>
+      </c>
+      <c r="E32" s="10"/>
       <c r="F32" s="29" t="s">
         <v>275</v>
       </c>
@@ -7668,7 +7773,7 @@
       </c>
       <c r="S32" s="36"/>
     </row>
-    <row r="33" spans="1:19" ht="409.5">
+    <row r="33" spans="1:19" ht="126">
       <c r="A33" s="10" t="s">
         <v>267</v>
       </c>
@@ -7679,7 +7784,7 @@
         <v>272</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>273</v>
+        <v>472</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="29" t="s">
@@ -7717,7 +7822,7 @@
       </c>
       <c r="S33" s="36"/>
     </row>
-    <row r="34" spans="1:19" ht="409.5">
+    <row r="34" spans="1:19" ht="126">
       <c r="A34" s="10" t="s">
         <v>268</v>
       </c>
@@ -7728,7 +7833,7 @@
         <v>272</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>273</v>
+        <v>472</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="29" t="s">
@@ -7768,7 +7873,7 @@
       </c>
       <c r="S34" s="36"/>
     </row>
-    <row r="35" spans="1:19" ht="409.5">
+    <row r="35" spans="1:19" ht="144">
       <c r="A35" s="12" t="s">
         <v>283</v>
       </c>
@@ -7779,7 +7884,7 @@
         <v>287</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>288</v>
+        <v>473</v>
       </c>
       <c r="E35" s="24"/>
       <c r="F35" s="30" t="s">
@@ -7819,7 +7924,7 @@
       </c>
       <c r="S35" s="36"/>
     </row>
-    <row r="36" spans="1:19" ht="409.5">
+    <row r="36" spans="1:19" ht="144">
       <c r="A36" s="12" t="s">
         <v>284</v>
       </c>
@@ -7830,7 +7935,7 @@
         <v>287</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>288</v>
+        <v>473</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="30" t="s">
@@ -7870,7 +7975,7 @@
       </c>
       <c r="S36" s="36"/>
     </row>
-    <row r="37" spans="1:19" ht="409.5">
+    <row r="37" spans="1:19" ht="198">
       <c r="A37" s="10" t="s">
         <v>294</v>
       </c>
@@ -7923,7 +8028,7 @@
       </c>
       <c r="S37" s="17"/>
     </row>
-    <row r="38" spans="1:19" ht="409.5">
+    <row r="38" spans="1:19" ht="252">
       <c r="A38" s="10" t="s">
         <v>121</v>
       </c>
@@ -7976,7 +8081,7 @@
       </c>
       <c r="S38" s="17"/>
     </row>
-    <row r="39" spans="1:19" ht="409.5">
+    <row r="39" spans="1:19" ht="108">
       <c r="A39" s="10" t="s">
         <v>295</v>
       </c>
@@ -7990,7 +8095,7 @@
         <v>308</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>309</v>
+        <v>479</v>
       </c>
       <c r="F39" s="29" t="s">
         <v>311</v>
@@ -8029,7 +8134,7 @@
       </c>
       <c r="S39" s="17"/>
     </row>
-    <row r="40" spans="1:19" ht="409.5">
+    <row r="40" spans="1:19" ht="198">
       <c r="A40" s="10" t="s">
         <v>296</v>
       </c>
@@ -8080,7 +8185,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="409.5">
+    <row r="41" spans="1:19" ht="126">
       <c r="A41" s="15" t="s">
         <v>297</v>
       </c>
@@ -8088,13 +8193,13 @@
         <v>303</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>308</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>309</v>
+        <v>480</v>
       </c>
       <c r="F41" s="29" t="s">
         <v>311</v>
@@ -8133,7 +8238,7 @@
       </c>
       <c r="S41" s="17"/>
     </row>
-    <row r="42" spans="1:19" ht="409.5">
+    <row r="42" spans="1:19" ht="252">
       <c r="A42" s="10" t="s">
         <v>298</v>
       </c>
@@ -8141,7 +8246,7 @@
         <v>304</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>308</v>
@@ -8184,7 +8289,7 @@
       </c>
       <c r="S42" s="18"/>
     </row>
-    <row r="43" spans="1:19" ht="375">
+    <row r="43" spans="1:19" ht="72">
       <c r="A43" s="12" t="s">
         <v>330</v>
       </c>
@@ -8195,11 +8300,9 @@
         <v>334</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>336</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="E43" s="12"/>
       <c r="F43" s="30" t="s">
         <v>337</v>
       </c>
@@ -8237,7 +8340,7 @@
       </c>
       <c r="S43" s="24"/>
     </row>
-    <row r="44" spans="1:19" ht="409.5">
+    <row r="44" spans="1:19" ht="72">
       <c r="A44" s="12" t="s">
         <v>331</v>
       </c>
@@ -8248,11 +8351,9 @@
         <v>334</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>336</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="E44" s="12"/>
       <c r="F44" s="30" t="s">
         <v>337</v>
       </c>
@@ -8292,7 +8393,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="409.5">
+    <row r="45" spans="1:19" ht="90">
       <c r="A45" s="10" t="s">
         <v>266</v>
       </c>
@@ -8303,7 +8404,7 @@
         <v>341</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>342</v>
+        <v>475</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="29" t="s">
@@ -8343,7 +8444,7 @@
       </c>
       <c r="S45" s="36"/>
     </row>
-    <row r="46" spans="1:19" ht="131.25">
+    <row r="46" spans="1:19" ht="108">
       <c r="A46" s="12" t="s">
         <v>347</v>
       </c>
@@ -8392,7 +8493,7 @@
       </c>
       <c r="S46" s="36"/>
     </row>
-    <row r="47" spans="1:19" ht="393.75">
+    <row r="47" spans="1:19" ht="54">
       <c r="A47" s="12" t="s">
         <v>348</v>
       </c>
@@ -8439,7 +8540,7 @@
       </c>
       <c r="S47" s="36"/>
     </row>
-    <row r="48" spans="1:19" ht="409.5">
+    <row r="48" spans="1:19" ht="90">
       <c r="A48" s="12" t="s">
         <v>349</v>
       </c>
@@ -8486,7 +8587,7 @@
       </c>
       <c r="S48" s="36"/>
     </row>
-    <row r="49" spans="1:19" ht="409.5">
+    <row r="49" spans="1:19" ht="144">
       <c r="A49" s="10" t="s">
         <v>358</v>
       </c>
@@ -8497,7 +8598,7 @@
         <v>360</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>361</v>
+        <v>476</v>
       </c>
       <c r="E49" s="10"/>
       <c r="F49" s="29" t="s">
@@ -8535,7 +8636,7 @@
       </c>
       <c r="S49" s="36"/>
     </row>
-    <row r="50" spans="1:19" ht="409.5">
+    <row r="50" spans="1:19" ht="108">
       <c r="A50" s="12" t="s">
         <v>365</v>
       </c>
@@ -8545,9 +8646,7 @@
       <c r="C50" s="12" t="s">
         <v>367</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>368</v>
-      </c>
+      <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="30" t="s">
         <v>369</v>
@@ -8584,7 +8683,7 @@
       </c>
       <c r="S50" s="36"/>
     </row>
-    <row r="51" spans="1:19" ht="409.5">
+    <row r="51" spans="1:19" ht="144">
       <c r="A51" s="16" t="s">
         <v>372</v>
       </c>
@@ -8595,7 +8694,7 @@
         <v>378</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>379</v>
+        <v>477</v>
       </c>
       <c r="E51" s="10"/>
       <c r="F51" s="10" t="s">
@@ -8639,13 +8738,17 @@
         <v>385</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="75">
+    <row r="52" spans="1:19" ht="72">
       <c r="A52" s="10" t="s">
         <v>373</v>
       </c>
       <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
+      <c r="C52" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>477</v>
+      </c>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
@@ -8662,13 +8765,17 @@
       <c r="R52" s="10"/>
       <c r="S52" s="17"/>
     </row>
-    <row r="53" spans="1:19" ht="112.5">
+    <row r="53" spans="1:19" ht="72">
       <c r="A53" s="10" t="s">
         <v>374</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
+      <c r="C53" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>477</v>
+      </c>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
@@ -8685,13 +8792,17 @@
       <c r="R53" s="10"/>
       <c r="S53" s="17"/>
     </row>
-    <row r="54" spans="1:19" ht="18.75">
+    <row r="54" spans="1:19" ht="72">
       <c r="A54" s="17" t="s">
         <v>375</v>
       </c>
       <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
+      <c r="C54" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>477</v>
+      </c>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -8708,13 +8819,17 @@
       <c r="R54" s="18"/>
       <c r="S54" s="18"/>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" ht="72">
       <c r="A55" s="18" t="s">
         <v>376</v>
       </c>
       <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
+      <c r="C55" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>477</v>
+      </c>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
@@ -8731,18 +8846,18 @@
       <c r="R55" s="18"/>
       <c r="S55" s="18"/>
     </row>
-    <row r="56" spans="1:19" ht="409.5">
+    <row r="56" spans="1:19" ht="342">
       <c r="A56" s="12" t="s">
         <v>386</v>
       </c>
       <c r="B56" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>389</v>
+      <c r="C56" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>477</v>
       </c>
       <c r="E56" s="25"/>
       <c r="F56" s="12" t="s">
@@ -8780,7 +8895,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="409.5">
+    <row r="57" spans="1:19" ht="396">
       <c r="A57" s="19" t="s">
         <v>394</v>
       </c>
@@ -8791,11 +8906,9 @@
         <v>402</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>404</v>
-      </c>
+        <v>478</v>
+      </c>
+      <c r="E57" s="10"/>
       <c r="F57" s="29" t="s">
         <v>405</v>
       </c>
@@ -8837,7 +8950,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="409.5">
+    <row r="58" spans="1:19" ht="288">
       <c r="A58" s="19" t="s">
         <v>395</v>
       </c>
@@ -8847,12 +8960,10 @@
       <c r="C58" s="22" t="s">
         <v>402</v>
       </c>
-      <c r="D58" s="22" t="s">
-        <v>403</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>404</v>
-      </c>
+      <c r="D58" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="E58" s="22"/>
       <c r="F58" s="29" t="s">
         <v>405</v>
       </c>
@@ -8892,15 +9003,19 @@
       </c>
       <c r="S58" s="17"/>
     </row>
-    <row r="59" spans="1:19" ht="409.5">
+    <row r="59" spans="1:19" ht="198">
       <c r="A59" s="19" t="s">
         <v>396</v>
       </c>
       <c r="B59" s="22" t="s">
         <v>400</v>
       </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
+      <c r="C59" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>478</v>
+      </c>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
@@ -8937,15 +9052,19 @@
       </c>
       <c r="S59" s="17"/>
     </row>
-    <row r="60" spans="1:19" ht="409.5">
+    <row r="60" spans="1:19" ht="342">
       <c r="A60" s="19" t="s">
         <v>397</v>
       </c>
       <c r="B60" s="22" t="s">
         <v>401</v>
       </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
+      <c r="C60" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>478</v>
+      </c>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
@@ -8980,7 +9099,7 @@
       </c>
       <c r="S60" s="18"/>
     </row>
-    <row r="61" spans="1:19" ht="409.5">
+    <row r="61" spans="1:19" ht="252">
       <c r="A61" s="12" t="s">
         <v>418</v>
       </c>
@@ -8990,8 +9109,8 @@
       <c r="C61" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="D61" s="24" t="s">
-        <v>429</v>
+      <c r="D61" s="12" t="s">
+        <v>482</v>
       </c>
       <c r="E61" s="25"/>
       <c r="F61" s="30" t="s">
@@ -9031,15 +9150,19 @@
       </c>
       <c r="S61" s="24"/>
     </row>
-    <row r="62" spans="1:19" ht="409.5">
+    <row r="62" spans="1:19" ht="180">
       <c r="A62" s="12" t="s">
         <v>419</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
+      <c r="C62" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>482</v>
+      </c>
       <c r="E62" s="12"/>
       <c r="F62" s="30" t="s">
         <v>430</v>
@@ -9080,15 +9203,19 @@
         <v>442</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="409.5">
+    <row r="63" spans="1:19" ht="216">
       <c r="A63" s="12" t="s">
         <v>420</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
+      <c r="C63" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>482</v>
+      </c>
       <c r="E63" s="12"/>
       <c r="F63" s="30" t="s">
         <v>430</v>
@@ -9127,15 +9254,19 @@
       </c>
       <c r="S63" s="24"/>
     </row>
-    <row r="64" spans="1:19" ht="409.5">
+    <row r="64" spans="1:19" ht="162">
       <c r="A64" s="12" t="s">
         <v>421</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
+      <c r="C64" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>482</v>
+      </c>
       <c r="E64" s="25"/>
       <c r="F64" s="24" t="s">
         <v>430</v>
@@ -9172,15 +9303,19 @@
       </c>
       <c r="S64" s="25"/>
     </row>
-    <row r="65" spans="1:19" ht="409.5">
+    <row r="65" spans="1:19" ht="234">
       <c r="A65" s="12" t="s">
         <v>422</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
+      <c r="C65" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>482</v>
+      </c>
       <c r="E65" s="25"/>
       <c r="F65" s="24" t="s">
         <v>430</v>
@@ -9219,7 +9354,7 @@
       </c>
       <c r="S65" s="25"/>
     </row>
-    <row r="66" spans="1:19" ht="409.5">
+    <row r="66" spans="1:19" ht="108">
       <c r="A66" s="10" t="s">
         <v>443</v>
       </c>
@@ -9232,9 +9367,7 @@
       <c r="D66" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="E66" s="10" t="s">
-        <v>166</v>
-      </c>
+      <c r="E66" s="10"/>
       <c r="F66" s="32" t="s">
         <v>450</v>
       </c>
@@ -9276,7 +9409,7 @@
       </c>
       <c r="S66" s="17"/>
     </row>
-    <row r="67" spans="1:19" ht="409.5">
+    <row r="67" spans="1:19" ht="270">
       <c r="A67" s="10" t="s">
         <v>444</v>
       </c>
@@ -9289,9 +9422,7 @@
       <c r="D67" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="E67" s="10" t="s">
-        <v>166</v>
-      </c>
+      <c r="E67" s="10"/>
       <c r="F67" s="32" t="s">
         <v>450</v>
       </c>
@@ -9333,7 +9464,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="409.5">
+    <row r="68" spans="1:19" ht="108">
       <c r="A68" s="10" t="s">
         <v>445</v>
       </c>
@@ -9346,9 +9477,7 @@
       <c r="D68" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="E68" s="10" t="s">
-        <v>166</v>
-      </c>
+      <c r="E68" s="10"/>
       <c r="F68" s="32" t="s">
         <v>451</v>
       </c>
@@ -9415,6 +9544,11 @@
     <hyperlink ref="F68" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>